<commit_message>
Assignment and Publishing of Locker Allocations
</commit_message>
<xml_diff>
--- a/test/data/Lockers.xlsx
+++ b/test/data/Lockers.xlsx
@@ -1,37 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ThisI\Desktop\cuslockers\test\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B02CA56B-CAA5-4FEC-8BD6-6808411033FE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5038252E-A29C-4EFD-B377-D16BC09302BD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Lockers" sheetId="1" r:id="rId1"/>
+    <sheet name="Basement" sheetId="1" r:id="rId1"/>
     <sheet name="Second Floor" sheetId="2" r:id="rId2"/>
     <sheet name="Third Floor" sheetId="3" r:id="rId3"/>
     <sheet name="Fourth Floor" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -342,10 +334,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
       <selection activeCell="E63" sqref="E63"/>
     </sheetView>
   </sheetViews>
@@ -672,7 +664,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A94"/>
   <sheetViews>
     <sheetView topLeftCell="A70" workbookViewId="0">
@@ -1157,7 +1149,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:A102"/>
   <sheetViews>
     <sheetView topLeftCell="A70" workbookViewId="0">
@@ -1682,7 +1674,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:A65"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>